<commit_message>
fix class prop, seq ban acc, req linkage
</commit_message>
<xml_diff>
--- a/Lab 1/Lab 1.3/Requirements Linkage Traceability Matrix.xlsx
+++ b/Lab 1/Lab 1.3/Requirements Linkage Traceability Matrix.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repository\SE357-Pratice class\Lab 1\Lab 1.3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F42FC44C-A286-458F-9C05-7ECCAE22380E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A96E3F3-9F3F-4BE5-BB6E-5C53DB9552C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{FC9513CD-CF22-4CA8-BE6D-50D44C571A54}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FC9513CD-CF22-4CA8-BE6D-50D44C571A54}"/>
   </bookViews>
   <sheets>
     <sheet name="RLTM" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="19">
   <si>
     <t>Requirement ID</t>
   </si>
@@ -479,15 +479,15 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -537,7 +537,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -567,7 +567,7 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -591,7 +591,7 @@
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -619,7 +619,7 @@
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -661,7 +661,7 @@
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -693,7 +693,7 @@
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -719,7 +719,7 @@
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -729,9 +729,7 @@
       <c r="C8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -747,7 +745,7 @@
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -775,7 +773,7 @@
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -803,7 +801,7 @@
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -831,7 +829,7 @@
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -863,7 +861,7 @@
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -893,7 +891,7 @@
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -923,7 +921,7 @@
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -949,7 +947,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>

</xml_diff>